<commit_message>
Updates Oct 2015 connection type stats - query was incorrect
</commit_message>
<xml_diff>
--- a/Documents/Connection Type By Country Oct 2015.xlsx
+++ b/Documents/Connection Type By Country Oct 2015.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$275</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$314</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="88">
   <si>
     <t>Aruba</t>
   </si>
@@ -275,16 +275,22 @@
     <t>SAE Combo (DC Fast Charge J1772)</t>
   </si>
   <si>
-    <t>Macedonia</t>
-  </si>
-  <si>
     <t>Serbia</t>
   </si>
   <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
     <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Reunion</t>
   </si>
 </sst>
 </file>
@@ -611,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C314"/>
+  <dimension ref="A1:C311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,10 +643,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -648,13 +654,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,10 +668,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,10 +679,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,10 +690,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,10 +701,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,10 +712,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
         <v>5</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,10 +723,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,10 +734,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,10 +745,10 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,13 +764,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>150</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,10 +778,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,10 +789,10 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,10 +800,10 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,10 +811,10 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,10 +822,10 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,7 +833,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -838,18 +844,18 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -860,7 +866,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -868,13 +874,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23">
-        <v>368</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,10 +888,10 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>127</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -896,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="C25">
-        <v>61</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,10 +910,10 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26">
-        <v>45</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,10 +921,10 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C27">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,10 +932,10 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,10 +943,10 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,7 +954,7 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C30">
         <v>8</v>
@@ -959,10 +965,10 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,10 +976,10 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -981,10 +987,10 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -992,10 +998,10 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,7 +1009,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1014,7 +1020,7 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1025,7 +1031,7 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1036,7 +1042,7 @@
         <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1044,18 +1050,18 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1066,21 +1072,21 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C41">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -1088,24 +1094,24 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C43">
-        <v>357</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,10 +1119,10 @@
         <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>656</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,10 +1130,10 @@
         <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,10 +1141,10 @@
         <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,10 +1152,10 @@
         <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,10 +1163,10 @@
         <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1168,10 +1174,10 @@
         <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1190,7 +1196,7 @@
         <v>24</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1201,7 +1207,7 @@
         <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1209,21 +1215,21 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>123</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1231,35 +1237,35 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C56">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1267,43 +1273,43 @@
         <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C60">
-        <v>115</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C61">
-        <v>81</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C62">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1311,10 +1317,10 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C63">
-        <v>17</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1322,10 +1328,10 @@
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C64">
-        <v>9</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,10 +1339,10 @@
         <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1344,10 +1350,10 @@
         <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1355,10 +1361,10 @@
         <v>28</v>
       </c>
       <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67">
         <v>9</v>
-      </c>
-      <c r="C67">
-        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1366,10 +1372,10 @@
         <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1377,43 +1383,43 @@
         <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C70">
-        <v>362</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C72">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1421,10 +1427,10 @@
         <v>29</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,10 +1438,10 @@
         <v>29</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1443,51 +1449,51 @@
         <v>29</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C76">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C77">
-        <v>150</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -1495,46 +1501,46 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C80">
-        <v>98</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B81" t="s">
         <v>3</v>
       </c>
       <c r="C81">
-        <v>64</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C82">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C83">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1542,10 +1548,10 @@
         <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1553,10 +1559,10 @@
         <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1564,10 +1570,10 @@
         <v>31</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1575,54 +1581,54 @@
         <v>31</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C88">
-        <v>216</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B89" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>159</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C90">
-        <v>53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C91">
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1630,10 +1636,10 @@
         <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>12</v>
+        <v>755</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1641,10 +1647,10 @@
         <v>33</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C93">
-        <v>10</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1652,10 +1658,10 @@
         <v>33</v>
       </c>
       <c r="B94" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C94">
-        <v>9</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,10 +1669,10 @@
         <v>33</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1674,10 +1680,10 @@
         <v>33</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1685,10 +1691,10 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1696,10 +1702,10 @@
         <v>33</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1707,10 +1713,10 @@
         <v>33</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1718,10 +1724,10 @@
         <v>33</v>
       </c>
       <c r="B100" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1729,54 +1735,54 @@
         <v>33</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B102" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C102">
-        <v>3882</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C103">
-        <v>1590</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B104" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C104">
-        <v>407</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C105">
-        <v>383</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1784,10 +1790,10 @@
         <v>35</v>
       </c>
       <c r="B106" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C106">
-        <v>264</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1795,10 +1801,10 @@
         <v>35</v>
       </c>
       <c r="B107" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C107">
-        <v>204</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1806,10 +1812,10 @@
         <v>35</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C108">
-        <v>45</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1817,10 +1823,10 @@
         <v>35</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C109">
-        <v>32</v>
+        <v>381</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,10 +1834,10 @@
         <v>35</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C110">
-        <v>22</v>
+        <v>256</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1839,10 +1845,10 @@
         <v>35</v>
       </c>
       <c r="B111" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C111">
-        <v>14</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1850,10 +1856,10 @@
         <v>35</v>
       </c>
       <c r="B112" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C112">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1861,10 +1867,10 @@
         <v>35</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C113">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1872,10 +1878,10 @@
         <v>35</v>
       </c>
       <c r="B114" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C114">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1883,10 +1889,10 @@
         <v>35</v>
       </c>
       <c r="B115" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1894,10 +1900,10 @@
         <v>35</v>
       </c>
       <c r="B116" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C116">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1905,10 +1911,10 @@
         <v>35</v>
       </c>
       <c r="B117" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1916,10 +1922,10 @@
         <v>35</v>
       </c>
       <c r="B118" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,40 +1933,40 @@
         <v>35</v>
       </c>
       <c r="B119" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B120" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C120">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B121" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B122" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -1968,46 +1974,46 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B123" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C123">
-        <v>186</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B124" t="s">
         <v>3</v>
       </c>
       <c r="C124">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B125" t="s">
         <v>17</v>
       </c>
       <c r="C125">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B126" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C126">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2015,10 +2021,10 @@
         <v>39</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C127">
-        <v>2</v>
+        <v>186</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,10 +2032,10 @@
         <v>39</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C128">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2037,10 +2043,10 @@
         <v>39</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C129">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2048,10 +2054,10 @@
         <v>39</v>
       </c>
       <c r="B130" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C130">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2059,54 +2065,54 @@
         <v>39</v>
       </c>
       <c r="B131" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C131">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B132" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C132">
-        <v>70</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B133" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C133">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B134" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C134">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B135" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C135">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2114,10 +2120,10 @@
         <v>40</v>
       </c>
       <c r="B136" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C136">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2125,65 +2131,65 @@
         <v>40</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C138">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B139" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C139">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B140" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C140">
-        <v>288</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B141" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C141">
-        <v>85</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B142" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C142">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,10 +2197,10 @@
         <v>42</v>
       </c>
       <c r="B143" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C143">
-        <v>3</v>
+        <v>287</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,10 +2208,10 @@
         <v>42</v>
       </c>
       <c r="B144" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,10 +2219,10 @@
         <v>42</v>
       </c>
       <c r="B145" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C145">
-        <v>2</v>
+        <v>80</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,10 +2230,10 @@
         <v>42</v>
       </c>
       <c r="B146" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,40 +2241,40 @@
         <v>42</v>
       </c>
       <c r="B147" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B148" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C148">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B149" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B150" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -2276,35 +2282,35 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B151" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C151">
-        <v>467</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B152" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C152">
-        <v>257</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B153" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C153">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,10 +2318,10 @@
         <v>45</v>
       </c>
       <c r="B154" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C154">
-        <v>13</v>
+        <v>358</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,10 +2329,10 @@
         <v>45</v>
       </c>
       <c r="B155" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C155">
-        <v>13</v>
+        <v>186</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,10 +2340,10 @@
         <v>45</v>
       </c>
       <c r="B156" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C156">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,10 +2351,10 @@
         <v>45</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C157">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,10 +2362,10 @@
         <v>45</v>
       </c>
       <c r="B158" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C158">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,10 +2373,10 @@
         <v>45</v>
       </c>
       <c r="B159" t="s">
+        <v>12</v>
+      </c>
+      <c r="C159">
         <v>11</v>
-      </c>
-      <c r="C159">
-        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2378,10 +2384,10 @@
         <v>45</v>
       </c>
       <c r="B160" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2389,10 +2395,10 @@
         <v>45</v>
       </c>
       <c r="B161" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,10 +2406,10 @@
         <v>45</v>
       </c>
       <c r="B162" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="C162">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,10 +2417,10 @@
         <v>45</v>
       </c>
       <c r="B163" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2430,35 +2436,35 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B165" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C165">
-        <v>1275</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B166" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C166">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B167" t="s">
         <v>10</v>
       </c>
       <c r="C167">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2466,10 +2472,10 @@
         <v>46</v>
       </c>
       <c r="B168" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C168">
-        <v>8</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,10 +2483,10 @@
         <v>46</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C169">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,32 +2494,32 @@
         <v>46</v>
       </c>
       <c r="B170" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C170">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B171" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C171">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B172" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C172">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2521,10 +2527,10 @@
         <v>49</v>
       </c>
       <c r="B173" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C173">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2532,32 +2538,32 @@
         <v>49</v>
       </c>
       <c r="B174" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C174">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B175" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C175">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B176" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C176">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,10 +2571,10 @@
         <v>50</v>
       </c>
       <c r="B177" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C177">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,10 +2582,10 @@
         <v>50</v>
       </c>
       <c r="B178" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C178">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2587,10 +2593,10 @@
         <v>50</v>
       </c>
       <c r="B179" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C179">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2598,32 +2604,32 @@
         <v>50</v>
       </c>
       <c r="B180" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C180">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B181" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C181">
-        <v>55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B182" t="s">
         <v>17</v>
       </c>
       <c r="C182">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2631,10 +2637,10 @@
         <v>51</v>
       </c>
       <c r="B183" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C183">
-        <v>1</v>
+        <v>55</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2642,10 +2648,10 @@
         <v>51</v>
       </c>
       <c r="B184" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C184">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2653,10 +2659,10 @@
         <v>51</v>
       </c>
       <c r="B185" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C185">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2664,7 +2670,7 @@
         <v>51</v>
       </c>
       <c r="B186" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -2675,7 +2681,7 @@
         <v>51</v>
       </c>
       <c r="B187" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -2683,10 +2689,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B188" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -2694,10 +2700,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B189" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C189">
         <v>1</v>
@@ -2705,13 +2711,13 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B190" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C190">
-        <v>99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2719,21 +2725,21 @@
         <v>53</v>
       </c>
       <c r="B191" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C191">
-        <v>2</v>
+        <v>99</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B192" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C192">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -2741,21 +2747,21 @@
         <v>54</v>
       </c>
       <c r="B193" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C193">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B194" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C194">
-        <v>9877</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2763,10 +2769,10 @@
         <v>55</v>
       </c>
       <c r="B195" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C195">
-        <v>133</v>
+        <v>9831</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2774,10 +2780,10 @@
         <v>55</v>
       </c>
       <c r="B196" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C196">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2785,10 +2791,10 @@
         <v>55</v>
       </c>
       <c r="B197" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C197">
-        <v>72</v>
+        <v>128</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -2796,10 +2802,10 @@
         <v>55</v>
       </c>
       <c r="B198" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C198">
-        <v>6</v>
+        <v>72</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -2810,7 +2816,7 @@
         <v>7</v>
       </c>
       <c r="C199">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2818,10 +2824,10 @@
         <v>55</v>
       </c>
       <c r="B200" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C200">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,10 +2835,10 @@
         <v>55</v>
       </c>
       <c r="B201" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C201">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -2840,7 +2846,7 @@
         <v>55</v>
       </c>
       <c r="B202" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -2848,13 +2854,13 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B203" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C203">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -2862,10 +2868,10 @@
         <v>56</v>
       </c>
       <c r="B204" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C204">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -2873,7 +2879,7 @@
         <v>56</v>
       </c>
       <c r="B205" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -2881,10 +2887,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B206" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -2892,13 +2898,13 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B207" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C207">
-        <v>1145</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -2906,10 +2912,10 @@
         <v>58</v>
       </c>
       <c r="B208" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C208">
-        <v>178</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -2917,10 +2923,10 @@
         <v>58</v>
       </c>
       <c r="B209" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C209">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -2928,10 +2934,10 @@
         <v>58</v>
       </c>
       <c r="B210" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C210">
-        <v>19</v>
+        <v>161</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -2939,10 +2945,10 @@
         <v>58</v>
       </c>
       <c r="B211" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C211">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -2950,10 +2956,10 @@
         <v>58</v>
       </c>
       <c r="B212" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C212">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -2961,10 +2967,10 @@
         <v>58</v>
       </c>
       <c r="B213" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="C213">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -2972,10 +2978,10 @@
         <v>58</v>
       </c>
       <c r="B214" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="C214">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -2983,10 +2989,10 @@
         <v>58</v>
       </c>
       <c r="B215" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C215">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -3005,10 +3011,10 @@
         <v>58</v>
       </c>
       <c r="B217" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C217">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -3016,10 +3022,10 @@
         <v>58</v>
       </c>
       <c r="B218" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C218">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -3030,7 +3036,7 @@
         <v>3</v>
       </c>
       <c r="C219">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -3049,10 +3055,10 @@
         <v>60</v>
       </c>
       <c r="B221" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C221">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -3060,10 +3066,10 @@
         <v>60</v>
       </c>
       <c r="B222" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C222">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -3079,13 +3085,13 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B224" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>413</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -3093,10 +3099,10 @@
         <v>61</v>
       </c>
       <c r="B225" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C225">
-        <v>400</v>
+        <v>41</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -3104,21 +3110,21 @@
         <v>61</v>
       </c>
       <c r="B226" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C226">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B227" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C227">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -3126,18 +3132,18 @@
         <v>62</v>
       </c>
       <c r="B228" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C228">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B229" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -3145,7 +3151,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B230" t="s">
         <v>3</v>
@@ -3159,10 +3165,10 @@
         <v>63</v>
       </c>
       <c r="B231" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C231">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -3170,10 +3176,10 @@
         <v>63</v>
       </c>
       <c r="B232" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C232">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -3184,7 +3190,7 @@
         <v>11</v>
       </c>
       <c r="C233">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -3195,7 +3201,7 @@
         <v>18</v>
       </c>
       <c r="C234">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -3206,51 +3212,51 @@
         <v>16</v>
       </c>
       <c r="C235">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B236" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C236">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B237" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C237">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B238" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C238">
-        <v>5</v>
+        <v>224</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B239" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C239">
-        <v>3</v>
+        <v>101</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -3258,10 +3264,10 @@
         <v>66</v>
       </c>
       <c r="B240" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C240">
-        <v>224</v>
+        <v>43</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -3269,10 +3275,10 @@
         <v>66</v>
       </c>
       <c r="B241" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C241">
-        <v>101</v>
+        <v>43</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -3280,10 +3286,10 @@
         <v>66</v>
       </c>
       <c r="B242" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C242">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -3291,10 +3297,10 @@
         <v>66</v>
       </c>
       <c r="B243" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="C243">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -3302,10 +3308,10 @@
         <v>66</v>
       </c>
       <c r="B244" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="C244">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -3313,10 +3319,10 @@
         <v>66</v>
       </c>
       <c r="B245" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C245">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -3324,10 +3330,10 @@
         <v>66</v>
       </c>
       <c r="B246" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C246">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -3335,43 +3341,43 @@
         <v>66</v>
       </c>
       <c r="B247" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C247">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B248" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C248">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B249" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C249">
-        <v>1</v>
+        <v>224</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B250" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C250">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -3379,10 +3385,10 @@
         <v>68</v>
       </c>
       <c r="B251" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C251">
-        <v>223</v>
+        <v>75</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -3390,10 +3396,10 @@
         <v>68</v>
       </c>
       <c r="B252" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C252">
-        <v>81</v>
+        <v>15</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -3401,10 +3407,10 @@
         <v>68</v>
       </c>
       <c r="B253" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C253">
-        <v>76</v>
+        <v>10</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -3412,10 +3418,10 @@
         <v>68</v>
       </c>
       <c r="B254" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C254">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -3423,10 +3429,10 @@
         <v>68</v>
       </c>
       <c r="B255" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C255">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -3434,10 +3440,10 @@
         <v>68</v>
       </c>
       <c r="B256" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C256">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -3445,10 +3451,10 @@
         <v>68</v>
       </c>
       <c r="B257" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C257">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -3456,10 +3462,10 @@
         <v>68</v>
       </c>
       <c r="B258" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C258">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -3475,24 +3481,24 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B260" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C260">
-        <v>1</v>
+        <v>197</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B261" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C261">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -3500,10 +3506,10 @@
         <v>69</v>
       </c>
       <c r="B262" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C262">
-        <v>203</v>
+        <v>9</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -3511,10 +3517,10 @@
         <v>69</v>
       </c>
       <c r="B263" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C263">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -3522,10 +3528,10 @@
         <v>69</v>
       </c>
       <c r="B264" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C264">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -3533,10 +3539,10 @@
         <v>69</v>
       </c>
       <c r="B265" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C265">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -3544,10 +3550,10 @@
         <v>69</v>
       </c>
       <c r="B266" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C266">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -3555,10 +3561,10 @@
         <v>69</v>
       </c>
       <c r="B267" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C267">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -3566,10 +3572,10 @@
         <v>69</v>
       </c>
       <c r="B268" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C268">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -3577,10 +3583,10 @@
         <v>69</v>
       </c>
       <c r="B269" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C269">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -3588,10 +3594,10 @@
         <v>69</v>
       </c>
       <c r="B270" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C270">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -3599,29 +3605,29 @@
         <v>69</v>
       </c>
       <c r="B271" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C271">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B272" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C272">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B273" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C273">
         <v>1</v>
@@ -3629,46 +3635,46 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B274" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C274">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B275" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C275">
-        <v>1</v>
+        <v>2852</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B276" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C276">
-        <v>1</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B277" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C277">
-        <v>1</v>
+        <v>561</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -3676,10 +3682,10 @@
         <v>71</v>
       </c>
       <c r="B278" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C278">
-        <v>2917</v>
+        <v>482</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -3687,10 +3693,10 @@
         <v>71</v>
       </c>
       <c r="B279" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C279">
-        <v>1039</v>
+        <v>373</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -3698,10 +3704,10 @@
         <v>71</v>
       </c>
       <c r="B280" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C280">
-        <v>574</v>
+        <v>125</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -3709,10 +3715,10 @@
         <v>71</v>
       </c>
       <c r="B281" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C281">
-        <v>386</v>
+        <v>39</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -3720,10 +3726,10 @@
         <v>71</v>
       </c>
       <c r="B282" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C282">
-        <v>124</v>
+        <v>13</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -3731,10 +3737,10 @@
         <v>71</v>
       </c>
       <c r="B283" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C283">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -3742,10 +3748,10 @@
         <v>71</v>
       </c>
       <c r="B284" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C284">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -3753,10 +3759,10 @@
         <v>71</v>
       </c>
       <c r="B285" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C285">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -3764,10 +3770,10 @@
         <v>71</v>
       </c>
       <c r="B286" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C286">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -3775,10 +3781,10 @@
         <v>71</v>
       </c>
       <c r="B287" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C287">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -3786,10 +3792,10 @@
         <v>71</v>
       </c>
       <c r="B288" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C288">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,7 +3803,7 @@
         <v>71</v>
       </c>
       <c r="B289" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -3816,35 +3822,35 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B291" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C291">
-        <v>1</v>
+        <v>11291</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B292" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="C292">
-        <v>1</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B293" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C293">
-        <v>1</v>
+        <v>680</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -3852,10 +3858,10 @@
         <v>72</v>
       </c>
       <c r="B294" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C294">
-        <v>11484</v>
+        <v>602</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -3863,10 +3869,10 @@
         <v>72</v>
       </c>
       <c r="B295" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C295">
-        <v>1751</v>
+        <v>220</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,10 +3880,10 @@
         <v>72</v>
       </c>
       <c r="B296" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="C296">
-        <v>631</v>
+        <v>135</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,10 +3891,10 @@
         <v>72</v>
       </c>
       <c r="B297" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C297">
-        <v>613</v>
+        <v>57</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -3896,10 +3902,10 @@
         <v>72</v>
       </c>
       <c r="B298" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C298">
-        <v>243</v>
+        <v>44</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -3907,10 +3913,10 @@
         <v>72</v>
       </c>
       <c r="B299" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C299">
-        <v>141</v>
+        <v>43</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -3918,10 +3924,10 @@
         <v>72</v>
       </c>
       <c r="B300" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="C300">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -3929,10 +3935,10 @@
         <v>72</v>
       </c>
       <c r="B301" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="C301">
-        <v>44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -3940,10 +3946,10 @@
         <v>72</v>
       </c>
       <c r="B302" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="C302">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -3951,10 +3957,10 @@
         <v>72</v>
       </c>
       <c r="B303" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C303">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -3962,10 +3968,10 @@
         <v>72</v>
       </c>
       <c r="B304" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="C304">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -3973,10 +3979,10 @@
         <v>72</v>
       </c>
       <c r="B305" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="C305">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -3984,10 +3990,10 @@
         <v>72</v>
       </c>
       <c r="B306" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C306">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -3995,10 +4001,10 @@
         <v>72</v>
       </c>
       <c r="B307" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C307">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -4006,10 +4012,10 @@
         <v>72</v>
       </c>
       <c r="B308" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C308">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -4017,7 +4023,7 @@
         <v>72</v>
       </c>
       <c r="B309" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="C309">
         <v>1</v>
@@ -4028,7 +4034,7 @@
         <v>72</v>
       </c>
       <c r="B310" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="C310">
         <v>1</v>
@@ -4045,41 +4051,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>72</v>
-      </c>
-      <c r="B312" t="s">
-        <v>77</v>
-      </c>
-      <c r="C312">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
-        <v>72</v>
-      </c>
-      <c r="B313" t="s">
-        <v>76</v>
-      </c>
-      <c r="C313">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
-        <v>72</v>
-      </c>
-      <c r="B314" t="s">
-        <v>13</v>
-      </c>
-      <c r="C314">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C275"/>
+  <autoFilter ref="A1:C314"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>